<commit_message>
Preparation release 200 f4d5df795db3adbc63e64601ff3b946598a24f89
</commit_message>
<xml_diff>
--- a/369-préparation-publication-release-200/ig/CodeSystem-tddui-encounter-identifier.xlsx
+++ b/369-préparation-publication-release-200/ig/CodeSystem-tddui-encounter-identifier.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.0.0-ballot</t>
+    <t>2.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-18T15:57:04+00:00</t>
+    <t>2025-09-19T09:50:13+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>